<commit_message>
I deleted 2 of the libraries in fastq03.10.20 that were submitted for this spike in. This was a case where we had 2 spike in fastq files for a single sample (26a/b) due to a mishap with Index1s. I was instructed to delete these samples for the spike in  to simplify the database.
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_03.10.20.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_03.10.20.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1EB965-F441-D044-9CB5-71FD33AF8F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D87D9EF-23E1-F244-AF5E-24A5B8B49E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18400" yWindow="460" windowWidth="18900" windowHeight="19660" xr2:uid="{A522515E-7FE3-F04A-A034-7C6A42931E3B}"/>
+    <workbookView xWindow="5200" yWindow="460" windowWidth="18900" windowHeight="19660" xr2:uid="{A522515E-7FE3-F04A-A034-7C6A42931E3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="56">
   <si>
     <t>libraryDate</t>
   </si>
@@ -199,18 +198,6 @@
   </si>
   <si>
     <t>Brent_40_GTAC40_SIC_Index2_07_GTACGGC_GAGTTGGT_S58_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>Brent_26a_GTAC26_SIC_Index2_07_TCAACTG_GAGTTGGT_S43_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>Brent_26b_GTAC27_SIC_Index2_07_TGTTTGT_GAGTTGGT_S44_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>26a</t>
-  </si>
-  <si>
-    <t>26b</t>
   </si>
   <si>
     <t>J.PLAGGENBERG</t>
@@ -649,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CA217D-0C43-0B40-A462-5F05C8B33EE8}">
-  <dimension ref="A1:Z85"/>
+  <dimension ref="A1:Z83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,7 +706,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -769,7 +756,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -804,7 +791,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -839,7 +826,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
@@ -874,7 +861,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -909,7 +896,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
@@ -944,7 +931,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3">
         <v>7</v>
@@ -979,7 +966,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
@@ -1014,7 +1001,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3">
         <v>9</v>
@@ -1049,7 +1036,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" s="3">
         <v>10</v>
@@ -1084,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3">
         <v>11</v>
@@ -1119,7 +1106,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" s="3">
         <v>12</v>
@@ -1154,7 +1141,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14" s="3">
         <v>13</v>
@@ -1189,7 +1176,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3">
         <v>14</v>
@@ -1224,7 +1211,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3">
         <v>15</v>
@@ -1259,7 +1246,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3">
         <v>16</v>
@@ -1294,7 +1281,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3">
         <v>17</v>
@@ -1329,7 +1316,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3">
         <v>18</v>
@@ -1364,7 +1351,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C20" s="3">
         <v>19</v>
@@ -1399,7 +1386,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3">
         <v>20</v>
@@ -1434,7 +1421,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3">
         <v>21</v>
@@ -1469,7 +1456,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3">
         <v>22</v>
@@ -1504,7 +1491,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3">
         <v>23</v>
@@ -1539,7 +1526,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3">
         <v>24</v>
@@ -1574,7 +1561,7 @@
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3">
         <v>25</v>
@@ -1609,10 +1596,10 @@
         <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="C27" s="3">
+        <v>27</v>
       </c>
       <c r="D27" s="4">
         <v>4271</v>
@@ -1627,16 +1614,16 @@
         <v>13</v>
       </c>
       <c r="I27" s="18">
-        <v>6.46</v>
+        <v>5.9</v>
       </c>
       <c r="J27" s="14">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="K27" s="15">
-        <v>23382</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>55</v>
+        <v>1.6949152542372881</v>
+      </c>
+      <c r="K27" s="19">
+        <v>33823</v>
+      </c>
+      <c r="L27" s="20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -1644,10 +1631,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="C28" s="3">
+        <v>28</v>
       </c>
       <c r="D28" s="4">
         <v>4271</v>
@@ -1662,16 +1649,16 @@
         <v>13</v>
       </c>
       <c r="I28" s="18">
-        <v>6.46</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="J28" s="14">
-        <v>0.78</v>
-      </c>
-      <c r="K28" s="15">
-        <v>12381</v>
-      </c>
-      <c r="L28" s="16" t="s">
-        <v>56</v>
+        <v>2.1691973969631233</v>
+      </c>
+      <c r="K28" s="19">
+        <v>31350</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1679,10 +1666,10 @@
         <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C29" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D29" s="4">
         <v>4271</v>
@@ -1697,16 +1684,16 @@
         <v>13</v>
       </c>
       <c r="I29" s="18">
-        <v>5.9</v>
+        <v>5.98</v>
       </c>
       <c r="J29" s="14">
-        <v>1.6949152542372881</v>
+        <v>1.6722408026755851</v>
       </c>
       <c r="K29" s="19">
-        <v>33823</v>
+        <v>28832</v>
       </c>
       <c r="L29" s="20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -1714,10 +1701,10 @@
         <v>15</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C30" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D30" s="4">
         <v>4271</v>
@@ -1732,16 +1719,16 @@
         <v>13</v>
       </c>
       <c r="I30" s="18">
-        <v>4.6100000000000003</v>
+        <v>7.77</v>
       </c>
       <c r="J30" s="14">
-        <v>2.1691973969631233</v>
+        <v>1.287001287001287</v>
       </c>
       <c r="K30" s="19">
-        <v>31350</v>
+        <v>29504</v>
       </c>
       <c r="L30" s="20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1749,10 +1736,10 @@
         <v>15</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C31" s="3">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D31" s="4">
         <v>4271</v>
@@ -1767,16 +1754,16 @@
         <v>13</v>
       </c>
       <c r="I31" s="18">
-        <v>5.98</v>
+        <v>1.43</v>
       </c>
       <c r="J31" s="14">
-        <v>1.6722408026755851</v>
+        <v>5</v>
       </c>
       <c r="K31" s="19">
-        <v>28832</v>
+        <v>24519</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1784,10 +1771,10 @@
         <v>15</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C32" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D32" s="4">
         <v>4271</v>
@@ -1802,16 +1789,16 @@
         <v>13</v>
       </c>
       <c r="I32" s="18">
-        <v>7.77</v>
+        <v>1.67</v>
       </c>
       <c r="J32" s="14">
-        <v>1.287001287001287</v>
+        <v>5</v>
       </c>
       <c r="K32" s="19">
-        <v>29504</v>
+        <v>49809</v>
       </c>
       <c r="L32" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -1819,10 +1806,10 @@
         <v>15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C33" s="3">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D33" s="4">
         <v>4271</v>
@@ -1837,16 +1824,16 @@
         <v>13</v>
       </c>
       <c r="I33" s="18">
-        <v>1.43</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="J33" s="14">
         <v>5</v>
       </c>
       <c r="K33" s="19">
-        <v>24519</v>
+        <v>696</v>
       </c>
       <c r="L33" s="20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -1854,10 +1841,10 @@
         <v>15</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C34" s="3">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D34" s="4">
         <v>4271</v>
@@ -1872,16 +1859,16 @@
         <v>13</v>
       </c>
       <c r="I34" s="18">
-        <v>1.67</v>
+        <v>1.23</v>
       </c>
       <c r="J34" s="14">
         <v>5</v>
       </c>
       <c r="K34" s="19">
-        <v>49809</v>
+        <v>16402</v>
       </c>
       <c r="L34" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -1889,10 +1876,10 @@
         <v>15</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C35" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D35" s="4">
         <v>4271</v>
@@ -1907,16 +1894,16 @@
         <v>13</v>
       </c>
       <c r="I35" s="18">
-        <v>0.27200000000000002</v>
+        <v>3.76</v>
       </c>
       <c r="J35" s="14">
-        <v>5</v>
+        <v>2.6595744680851063</v>
       </c>
       <c r="K35" s="19">
-        <v>696</v>
+        <v>34895</v>
       </c>
       <c r="L35" s="20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -1924,10 +1911,10 @@
         <v>15</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C36" s="3">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D36" s="4">
         <v>4271</v>
@@ -1942,16 +1929,16 @@
         <v>13</v>
       </c>
       <c r="I36" s="18">
-        <v>1.23</v>
+        <v>6.19</v>
       </c>
       <c r="J36" s="14">
-        <v>5</v>
+        <v>1.615508885298869</v>
       </c>
       <c r="K36" s="19">
-        <v>16402</v>
+        <v>30031</v>
       </c>
       <c r="L36" s="20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -1959,10 +1946,10 @@
         <v>15</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C37" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D37" s="4">
         <v>4271</v>
@@ -1977,16 +1964,16 @@
         <v>13</v>
       </c>
       <c r="I37" s="18">
-        <v>3.76</v>
-      </c>
-      <c r="J37" s="14">
-        <v>2.6595744680851063</v>
+        <v>13.1</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="K37" s="19">
-        <v>34895</v>
+        <v>37838</v>
       </c>
       <c r="L37" s="20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -1994,10 +1981,10 @@
         <v>15</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C38" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D38" s="4">
         <v>4271</v>
@@ -2012,16 +1999,16 @@
         <v>13</v>
       </c>
       <c r="I38" s="18">
-        <v>6.19</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="J38" s="14">
-        <v>1.615508885298869</v>
+        <v>2.2779043280182232</v>
       </c>
       <c r="K38" s="19">
-        <v>30031</v>
+        <v>37585</v>
       </c>
       <c r="L38" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2029,10 +2016,10 @@
         <v>15</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C39" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D39" s="4">
         <v>4271</v>
@@ -2047,16 +2034,16 @@
         <v>13</v>
       </c>
       <c r="I39" s="18">
-        <v>13.1</v>
-      </c>
-      <c r="J39" s="14" t="s">
-        <v>14</v>
+        <v>2.99</v>
+      </c>
+      <c r="J39" s="14">
+        <v>3.3444816053511701</v>
       </c>
       <c r="K39" s="19">
-        <v>37838</v>
+        <v>23651</v>
       </c>
       <c r="L39" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -2064,10 +2051,10 @@
         <v>15</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C40" s="3">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D40" s="4">
         <v>4271</v>
@@ -2082,92 +2069,40 @@
         <v>13</v>
       </c>
       <c r="I40" s="18">
-        <v>4.3899999999999997</v>
+        <v>2.42</v>
       </c>
       <c r="J40" s="14">
-        <v>2.2779043280182232</v>
+        <v>4.1322314049586781</v>
       </c>
       <c r="K40" s="19">
-        <v>37585</v>
+        <v>18735</v>
       </c>
       <c r="L40" s="20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="3">
-        <v>39</v>
-      </c>
-      <c r="D41" s="4">
-        <v>4271</v>
-      </c>
-      <c r="F41" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" t="s">
-        <v>13</v>
-      </c>
-      <c r="I41" s="18">
-        <v>2.99</v>
-      </c>
-      <c r="J41" s="14">
-        <v>3.3444816053511701</v>
-      </c>
-      <c r="K41" s="19">
-        <v>23651</v>
-      </c>
-      <c r="L41" s="20" t="s">
-        <v>53</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="16"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="3">
-        <v>40</v>
-      </c>
-      <c r="D42" s="4">
-        <v>4271</v>
-      </c>
-      <c r="F42" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" s="18">
-        <v>2.42</v>
-      </c>
-      <c r="J42" s="14">
-        <v>4.1322314049586781</v>
-      </c>
-      <c r="K42" s="19">
-        <v>18735</v>
-      </c>
-      <c r="L42" s="20" t="s">
-        <v>54</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+      <c r="D42" s="4"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="16"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="3"/>
       <c r="D43" s="4"/>
       <c r="I43" s="7"/>
       <c r="J43" s="8"/>
@@ -2195,8 +2130,9 @@
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
+      <c r="C46" s="3"/>
       <c r="D46" s="4"/>
-      <c r="I46" s="7"/>
+      <c r="I46" s="9"/>
       <c r="J46" s="8"/>
       <c r="K46" s="15"/>
       <c r="L46" s="16"/>
@@ -2205,7 +2141,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="D47" s="4"/>
-      <c r="I47" s="7"/>
+      <c r="I47" s="9"/>
       <c r="J47" s="8"/>
       <c r="K47" s="15"/>
       <c r="L47" s="16"/>
@@ -2213,7 +2149,6 @@
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="3"/>
       <c r="D48" s="4"/>
       <c r="I48" s="9"/>
       <c r="J48" s="8"/>
@@ -2232,6 +2167,7 @@
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
+      <c r="C50" s="3"/>
       <c r="D50" s="4"/>
       <c r="I50" s="9"/>
       <c r="J50" s="8"/>
@@ -2242,7 +2178,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="D51" s="4"/>
-      <c r="I51" s="9"/>
+      <c r="I51" s="10"/>
       <c r="J51" s="8"/>
       <c r="K51" s="15"/>
       <c r="L51" s="16"/>
@@ -2250,7 +2186,6 @@
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
-      <c r="C52" s="3"/>
       <c r="D52" s="4"/>
       <c r="I52" s="9"/>
       <c r="J52" s="8"/>
@@ -2261,7 +2196,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="D53" s="4"/>
-      <c r="I53" s="10"/>
+      <c r="I53" s="9"/>
       <c r="J53" s="8"/>
       <c r="K53" s="15"/>
       <c r="L53" s="16"/>
@@ -2278,6 +2213,7 @@
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
+      <c r="C55" s="3"/>
       <c r="D55" s="4"/>
       <c r="I55" s="9"/>
       <c r="J55" s="8"/>
@@ -2285,28 +2221,27 @@
       <c r="L55" s="16"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="4"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="8"/>
+      <c r="I56" s="13"/>
       <c r="K56" s="15"/>
       <c r="L56" s="16"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="3"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="4"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="8"/>
+      <c r="I57" s="13"/>
       <c r="K57" s="15"/>
       <c r="L57" s="16"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
-      <c r="C58" s="12"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="4"/>
       <c r="I58" s="13"/>
       <c r="K58" s="15"/>
@@ -2315,7 +2250,7 @@
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
+      <c r="C59" s="12"/>
       <c r="D59" s="4"/>
       <c r="I59" s="13"/>
       <c r="K59" s="15"/>
@@ -2333,7 +2268,7 @@
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="11"/>
       <c r="B61" s="11"/>
-      <c r="C61" s="12"/>
+      <c r="C61" s="11"/>
       <c r="D61" s="4"/>
       <c r="I61" s="13"/>
       <c r="K61" s="15"/>
@@ -2342,7 +2277,7 @@
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="11"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
+      <c r="C62" s="12"/>
       <c r="D62" s="4"/>
       <c r="I62" s="13"/>
       <c r="K62" s="15"/>
@@ -2360,7 +2295,7 @@
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="11"/>
       <c r="B64" s="11"/>
-      <c r="C64" s="12"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="4"/>
       <c r="I64" s="13"/>
       <c r="K64" s="15"/>
@@ -2369,7 +2304,7 @@
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="11"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
+      <c r="C65" s="12"/>
       <c r="D65" s="4"/>
       <c r="I65" s="13"/>
       <c r="K65" s="15"/>
@@ -2387,7 +2322,7 @@
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="4"/>
       <c r="I67" s="13"/>
       <c r="K67" s="15"/>
@@ -2396,7 +2331,7 @@
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
+      <c r="C68" s="12"/>
       <c r="D68" s="4"/>
       <c r="I68" s="13"/>
       <c r="K68" s="15"/>
@@ -2414,7 +2349,7 @@
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="11"/>
       <c r="B70" s="11"/>
-      <c r="C70" s="12"/>
+      <c r="C70" s="11"/>
       <c r="D70" s="4"/>
       <c r="I70" s="13"/>
       <c r="K70" s="15"/>
@@ -2423,7 +2358,7 @@
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
+      <c r="C71" s="12"/>
       <c r="D71" s="4"/>
       <c r="I71" s="13"/>
       <c r="K71" s="15"/>
@@ -2441,7 +2376,7 @@
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="11"/>
       <c r="B73" s="11"/>
-      <c r="C73" s="12"/>
+      <c r="C73" s="11"/>
       <c r="D73" s="4"/>
       <c r="I73" s="13"/>
       <c r="K73" s="15"/>
@@ -2450,7 +2385,7 @@
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="11"/>
       <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
+      <c r="C74" s="12"/>
       <c r="D74" s="4"/>
       <c r="I74" s="13"/>
       <c r="K74" s="15"/>
@@ -2468,7 +2403,7 @@
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="11"/>
       <c r="B76" s="11"/>
-      <c r="C76" s="12"/>
+      <c r="C76" s="11"/>
       <c r="D76" s="4"/>
       <c r="I76" s="13"/>
       <c r="K76" s="15"/>
@@ -2477,7 +2412,7 @@
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="11"/>
       <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
+      <c r="C77" s="12"/>
       <c r="D77" s="4"/>
       <c r="I77" s="13"/>
       <c r="K77" s="15"/>
@@ -2495,7 +2430,7 @@
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
-      <c r="C79" s="12"/>
+      <c r="C79" s="11"/>
       <c r="D79" s="4"/>
       <c r="I79" s="13"/>
       <c r="K79" s="15"/>
@@ -2504,48 +2439,30 @@
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="11"/>
       <c r="B80" s="11"/>
-      <c r="C80" s="11"/>
+      <c r="C80" s="12"/>
       <c r="D80" s="4"/>
       <c r="I80" s="13"/>
       <c r="K80" s="15"/>
       <c r="L80" s="16"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A81" s="11"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="4"/>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I81" s="13"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="16"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="4"/>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I82" s="13"/>
-      <c r="K82" s="15"/>
-      <c r="L82" s="16"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I83" s="13"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I84" s="13"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I85" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H42" xr:uid="{E4E9265D-9950-D34D-88D9-A900764ECD45}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H40" xr:uid="{E4E9265D-9950-D34D-88D9-A900764ECD45}">
       <formula1>"spikein, fullRNASeq, fullgDNASeq, fullChIPSeq, Rebalancing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42" xr:uid="{230D568A-431C-CE42-B4F2-604F39989810}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G40" xr:uid="{230D568A-431C-CE42-B4F2-604F39989810}">
       <formula1>"V3, Standard, Nano, MiniSeq, HighOutput, MidOutput"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F42" xr:uid="{1E46BD91-B032-CD4C-8815-6884616C34E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F40" xr:uid="{1E46BD91-B032-CD4C-8815-6884616C34E8}">
       <formula1>"MiSeq, MiniSeq, NextSeq"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>